<commit_message>
Normalizando con la primera forma normal (1FN)
</commit_message>
<xml_diff>
--- a/Normalización-part1.xlsx
+++ b/Normalización-part1.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JSamu\OneDrive\Documentos\BD - SQL\BD-SQL_Course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97967A2B-873A-4701-A586-B2B077BF6618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31F76C0-B7EC-43C7-91F7-33ED9CD5285A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{6362ABD5-D550-47A1-8806-3224D342D6E5}"/>
+    <workbookView xWindow="1350" yWindow="1515" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{6362ABD5-D550-47A1-8806-3224D342D6E5}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Modelo Desnormalizado" sheetId="1" r:id="rId1"/>
+    <sheet name="1FN" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="50">
   <si>
     <t>Venta</t>
   </si>
@@ -120,6 +121,72 @@
   </si>
   <si>
     <t>Micrófono</t>
+  </si>
+  <si>
+    <t>Juan</t>
+  </si>
+  <si>
+    <t>Perez</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gomez</t>
+  </si>
+  <si>
+    <t>Pedro</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Silva</t>
+  </si>
+  <si>
+    <t>Ana</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Perez</t>
+  </si>
+  <si>
+    <t>58-1</t>
+  </si>
+  <si>
+    <t>85-6</t>
+  </si>
+  <si>
+    <t>33-3</t>
+  </si>
+  <si>
+    <t>45-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calle 1 </t>
+  </si>
+  <si>
+    <t>Calle 2</t>
+  </si>
+  <si>
+    <t>Calle 3</t>
+  </si>
+  <si>
+    <t>Calle 4</t>
+  </si>
+  <si>
+    <t>Calle 5</t>
+  </si>
+  <si>
+    <t>Apellido</t>
+  </si>
+  <si>
+    <t>juan.perez@gmail.com</t>
+  </si>
+  <si>
+    <t>pedro.gomez@gmail.com</t>
+  </si>
+  <si>
+    <t>ana.silva@gmail.com</t>
+  </si>
+  <si>
+    <t>Número</t>
+  </si>
+  <si>
+    <t>CP</t>
   </si>
 </sst>
 </file>
@@ -127,9 +194,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="_-[$S/-280A]\ * #,##0.00_-;\-[$S/-280A]\ * #,##0.00_-;_-[$S/-280A]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-[$S/-280A]\ * #,##0.00_-;\-[$S/-280A]\ * #,##0.00_-;_-[$S/-280A]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,6 +221,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -186,7 +261,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -200,7 +275,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -538,10 +616,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8718452F-2995-4915-9880-12B25326597B}">
+  <sheetPr>
+    <tabColor theme="3"/>
+  </sheetPr>
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,4 +853,294 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2707EE7A-94FC-44C5-B783-D2A3BBBC8246}">
+  <dimension ref="A1:N6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="23.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>45292</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="2">
+        <v>918999043</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="2">
+        <v>3100</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="5">
+        <v>3000</v>
+      </c>
+      <c r="N2" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>45293</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="2">
+        <v>847776875</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="2">
+        <v>4100</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="5">
+        <v>6000</v>
+      </c>
+      <c r="N3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>45294</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="2">
+        <v>982761756</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" s="2">
+        <v>6400</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M4" s="5">
+        <v>700</v>
+      </c>
+      <c r="N4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>45295</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="2">
+        <v>938746162</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" s="2">
+        <v>6400</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="5">
+        <v>3000</v>
+      </c>
+      <c r="N5" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>45296</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="2">
+        <v>972647263</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="2">
+        <v>3920</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" s="5">
+        <v>700</v>
+      </c>
+      <c r="N6" s="2">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{7D627749-3FFC-4AC3-BEF5-74AA59EF7739}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{1CA4E672-8C11-4C71-9B92-CE41693D7D80}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{FEADF71C-8A23-4BA7-ABB0-C4AD3D2C20C4}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{CC3B483B-CB98-4942-AFB6-5D2BF83B0568}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{1F2ED31E-BDBB-4071-8007-83B1A9408AD2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>